<commit_message>
Criação de lista de presentes
</commit_message>
<xml_diff>
--- a/exemplo_dados_com_cpf_teste.xlsx
+++ b/exemplo_dados_com_cpf_teste.xlsx
@@ -483,7 +483,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>PRESENTE</t>
+          <t>AUSENTE</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>PRESENTE</t>
+          <t>AUSENTE</t>
         </is>
       </c>
     </row>

</xml_diff>